<commit_message>
chandra cleanup upto 19
</commit_message>
<xml_diff>
--- a/Chandrashekaran-annotations/BLIN_Q3_2019.xlsx
+++ b/Chandrashekaran-annotations/BLIN_Q3_2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vm056257\Downloads\Working\PEBU\ML\SubjECTive-QA\Chandrashekaran-annotations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976FBD99-10BE-45F7-AEC2-BBD1D93634EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903926AC-7DF5-46F6-918C-748294A91324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Asker</t>
   </si>
@@ -74,12 +74,6 @@
   </si>
   <si>
     <t>Right, well we are being approached by companies regularly, like more than once a month to review acquiring them. So we're seeing a lot of activity there and we able to integrate these businesses very quickly within three months. The company operates as a single company. So from an operational perspective, integrating another $2 million to $5 million business would not be a problem at all.That said, we want to establish a couple of quarters of showing bottom-line results. We think that that's going to be meaningful to investors. So our primary focus is operations right now is more of an opportunistic review of incoming acquisitions. We do think that strategic acquisitions are a key part of our future and in 2020 we'll make an even greater concerted effort to review opportunities.</t>
-  </si>
-  <si>
-    <t>Okay, well keep up the great work. It seems like the transformation is going as planned.</t>
-  </si>
-  <si>
-    <t>Great, thank you.</t>
   </si>
   <si>
     <t>Pearl Lee</t>
@@ -460,29 +454,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="88.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="88.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="89.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="93.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="89.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="93.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="88.140625" style="2"/>
+    <col min="10" max="10" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="88.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -514,7 +508,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -546,7 +540,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -578,7 +572,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -610,41 +604,41 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>2</v>
+      </c>
+      <c r="J5" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2">
-        <v>1</v>
-      </c>
-      <c r="H5" s="2">
-        <v>1</v>
-      </c>
-      <c r="I5" s="2">
-        <v>1</v>
-      </c>
-      <c r="J5" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
@@ -659,13 +653,13 @@
         <v>2</v>
       </c>
       <c r="F6" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="2">
         <v>2</v>
@@ -674,54 +668,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="2">
-        <v>2</v>
-      </c>
-      <c r="F7" s="2">
-        <v>2</v>
-      </c>
-      <c r="G7" s="2">
-        <v>1</v>
-      </c>
-      <c r="H7" s="2">
-        <v>1</v>
-      </c>
-      <c r="I7" s="2">
-        <v>2</v>
-      </c>
-      <c r="J7" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>